<commit_message>
annotations added, logs added, try catches organized
</commit_message>
<xml_diff>
--- a/Report_Request/report_request.xlsx
+++ b/Report_Request/report_request.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674DDE6A-13A0-4A42-BDCC-B833531295C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A0F747-F00D-4471-8C78-09A99A7919A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,14 +379,14 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>